<commit_message>
avg, min, and max of 100 sims
</commit_message>
<xml_diff>
--- a/examples/drinkingBaxter_rewards.xlsx
+++ b/examples/drinkingBaxter_rewards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nealg\git\assistive-gym\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FCE468B-611B-488C-90F7-A560F02244E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{064E484A-5501-4F46-A7FE-C434E86964AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{99BE97A3-FDC7-4D46-8608-05FC6D74F239}"/>
   </bookViews>
@@ -32,10 +32,32 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -63,8 +85,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -379,97 +402,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E91426-B366-4DF3-93FB-B8DD82305C49}">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>-110.824855284538</v>
       </c>
-      <c r="C1">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1">
         <f>AVERAGE(A:A)</f>
         <v>232.55648501525124</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>517.66766807530598</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>MAX(A:A)</f>
+        <v>567.10946987210696</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>420.37702980412598</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f>MIN(A:A)</f>
+        <v>-137.86292442774999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-92.141412681428093</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>128.11209983364199</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>139.76989107378</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-120.78782680731101</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>537.41346142217697</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>469.26943609022101</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-127.246468212293</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-92.652215076905406</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>436.76176913737299</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>258.61016498068898</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>133.88975309563401</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3.4585389832525402</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>473.93608696744298</v>
       </c>
@@ -900,15 +941,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F97311F71A5F6D46A9F867D8E429BF43" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="cd38647ae837cd19e76e6f39c8366a5b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c9e6236-0f58-4fd7-b0b1-11e21f2ac024" xmlns:ns4="79924f4f-d1b2-46f0-8945-c660332e2d28" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="24977efd720b8aba30c8ac495e10956a" ns3:_="" ns4:_="">
     <xsd:import namespace="2c9e6236-0f58-4fd7-b0b1-11e21f2ac024"/>
@@ -1119,6 +1151,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1126,14 +1167,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D1BBF-54FD-4456-9C57-DB78FB3F3B94}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41E378D5-E1DA-4A02-8C96-6178881B53B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1148,6 +1181,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E21D1BBF-54FD-4456-9C57-DB78FB3F3B94}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>